<commit_message>
cambio en cargas axiales de lm a aw funcional en ejemplos 4 y 5
</commit_message>
<xml_diff>
--- a/proyectos/ejemplo1/5/datos_generales.xlsx
+++ b/proyectos/ejemplo1/5/datos_generales.xlsx
@@ -9,8 +9,9 @@
   <sheets>
     <sheet name="kest" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="pcur" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="pcurg" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="dn_est" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="cargas nodales" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="pcurg" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="dn_est" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1052,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>9.99999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1060,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.920000000000019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1092,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>550.0879999999986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1100,7 +1101,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.355854680848614e-31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1108,7 +1109,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.919999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1140,7 +1141,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>114.912</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1149,6 +1150,126 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>9.99999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-1.920000000000019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>550.0879999999986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-1.355854680848614e-31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.919999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>114.912</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>